<commit_message>
Recruitment module done added root folder database
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -395,16 +395,16 @@
     <t>Recruitment  Module</t>
   </si>
   <si>
+    <t>5 Days</t>
+  </si>
+  <si>
+    <t>04-09-2023 to 09-09-2023</t>
+  </si>
+  <si>
+    <t>Holiday Management  Module</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not done </t>
-  </si>
-  <si>
-    <t>5 Days</t>
-  </si>
-  <si>
-    <t>04-09-2023 to 09-09-2023</t>
-  </si>
-  <si>
-    <t>Holiday Management  Module</t>
   </si>
   <si>
     <t>10-09-2023 to 12-09-2023</t>
@@ -2961,7 +2961,7 @@
   <sheetPr/>
   <dimension ref="A1:R114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
       <selection activeCell="I8" sqref="I8:I16"/>
     </sheetView>
   </sheetViews>
@@ -3417,14 +3417,14 @@
       <c r="G19" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="J19" s="32" t="s">
         <v>127</v>
-      </c>
-      <c r="J19" s="32" t="s">
-        <v>128</v>
       </c>
       <c r="K19" s="11"/>
     </row>
@@ -3443,8 +3443,8 @@
       <c r="G20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>126</v>
+      <c r="H20" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I20" s="36"/>
       <c r="J20" s="36"/>
@@ -3465,8 +3465,8 @@
       <c r="G21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="12" t="s">
-        <v>126</v>
+      <c r="H21" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I21" s="36"/>
       <c r="J21" s="36"/>
@@ -3487,8 +3487,8 @@
       <c r="G22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="12" t="s">
-        <v>126</v>
+      <c r="H22" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I22" s="36"/>
       <c r="J22" s="36"/>
@@ -3509,8 +3509,8 @@
       <c r="G23" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="12" t="s">
-        <v>126</v>
+      <c r="H23" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I23" s="36"/>
       <c r="J23" s="36"/>
@@ -3528,8 +3528,8 @@
       <c r="G24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="12" t="s">
-        <v>126</v>
+      <c r="H24" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I24" s="36"/>
       <c r="J24" s="36"/>
@@ -3549,8 +3549,8 @@
       <c r="G25" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H25" s="12" t="s">
-        <v>126</v>
+      <c r="H25" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I25" s="36"/>
       <c r="J25" s="36"/>
@@ -3570,8 +3570,8 @@
       <c r="G26" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>126</v>
+      <c r="H26" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
@@ -3606,7 +3606,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -3626,7 +3626,7 @@
         <v>55</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I29" s="32" t="s">
         <v>120</v>
@@ -3649,7 +3649,7 @@
         <v>56</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
@@ -3702,7 +3702,7 @@
         <v>58</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I33" s="32" t="s">
         <v>132</v>
@@ -3725,7 +3725,7 @@
         <v>59</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I34" s="36"/>
       <c r="J34" s="36"/>
@@ -3744,7 +3744,7 @@
         <v>60</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I35" s="36"/>
       <c r="J35" s="36"/>
@@ -3765,7 +3765,7 @@
         <v>61</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I36" s="36"/>
       <c r="J36" s="36"/>
@@ -3784,7 +3784,7 @@
         <v>62</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I37" s="36"/>
       <c r="J37" s="36"/>
@@ -3805,7 +3805,7 @@
         <v>63</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -3864,10 +3864,10 @@
         <v>65</v>
       </c>
       <c r="H41" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I41" s="32" t="s">
         <v>126</v>
-      </c>
-      <c r="I41" s="32" t="s">
-        <v>127</v>
       </c>
       <c r="J41" s="32" t="s">
         <v>135</v>
@@ -3889,7 +3889,7 @@
         <v>66</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I42" s="36"/>
       <c r="J42" s="36"/>
@@ -3910,7 +3910,7 @@
         <v>67</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I43" s="36"/>
       <c r="J43" s="36"/>
@@ -3931,7 +3931,7 @@
         <v>68</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I44" s="36"/>
       <c r="J44" s="36"/>
@@ -3952,7 +3952,7 @@
         <v>69</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I45" s="36"/>
       <c r="J45" s="36"/>
@@ -3973,7 +3973,7 @@
         <v>70</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I46" s="36"/>
       <c r="J46" s="36"/>
@@ -3994,7 +3994,7 @@
         <v>71</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I47" s="36"/>
       <c r="J47" s="36"/>
@@ -4015,7 +4015,7 @@
         <v>72</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I48" s="36"/>
       <c r="J48" s="36"/>
@@ -4036,7 +4036,7 @@
         <v>73</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
@@ -4095,7 +4095,7 @@
         <v>75</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I52" s="32" t="s">
         <v>132</v>
@@ -4120,7 +4120,7 @@
         <v>76</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I53" s="36"/>
       <c r="J53" s="36"/>
@@ -4141,7 +4141,7 @@
         <v>77</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I54" s="36"/>
       <c r="J54" s="36"/>
@@ -4162,7 +4162,7 @@
         <v>78</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I55" s="36"/>
       <c r="J55" s="36"/>
@@ -4183,7 +4183,7 @@
         <v>79</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I56" s="36"/>
       <c r="J56" s="36"/>
@@ -4204,7 +4204,7 @@
         <v>80</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I57" s="36"/>
       <c r="J57" s="36"/>
@@ -4225,7 +4225,7 @@
         <v>81</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
@@ -4331,7 +4331,7 @@
         <v>88</v>
       </c>
       <c r="H64" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I64" s="32" t="s">
         <v>132</v>
@@ -4354,7 +4354,7 @@
         <v>89</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
@@ -4373,7 +4373,7 @@
         <v>90</v>
       </c>
       <c r="H66" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I66" s="36"/>
       <c r="J66" s="36"/>
@@ -4392,7 +4392,7 @@
         <v>91</v>
       </c>
       <c r="H67" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I67" s="36"/>
       <c r="J67" s="36"/>
@@ -4411,7 +4411,7 @@
         <v>92</v>
       </c>
       <c r="H68" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I68" s="34"/>
       <c r="J68" s="34"/>
@@ -4464,10 +4464,10 @@
         <v>97</v>
       </c>
       <c r="H71" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="I71" s="32" t="s">
         <v>126</v>
-      </c>
-      <c r="I71" s="32" t="s">
-        <v>127</v>
       </c>
       <c r="J71" s="32" t="s">
         <v>142</v>
@@ -4487,7 +4487,7 @@
         <v>98</v>
       </c>
       <c r="H72" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I72" s="36"/>
       <c r="J72" s="36"/>
@@ -4506,7 +4506,7 @@
         <v>99</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I73" s="36"/>
       <c r="J73" s="36"/>
@@ -4525,7 +4525,7 @@
         <v>57</v>
       </c>
       <c r="H74" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I74" s="36"/>
       <c r="J74" s="36"/>
@@ -4544,7 +4544,7 @@
         <v>27</v>
       </c>
       <c r="H75" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I75" s="36"/>
       <c r="J75" s="36"/>
@@ -4563,7 +4563,7 @@
         <v>100</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I76" s="36"/>
       <c r="J76" s="36"/>
@@ -4582,7 +4582,7 @@
         <v>101</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I77" s="36"/>
       <c r="J77" s="36"/>
@@ -4601,7 +4601,7 @@
         <v>88</v>
       </c>
       <c r="H78" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I78" s="36"/>
       <c r="J78" s="36"/>
@@ -4620,7 +4620,7 @@
         <v>81</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I79" s="36"/>
       <c r="J79" s="36"/>
@@ -4639,7 +4639,7 @@
         <v>44</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I80" s="36"/>
       <c r="J80" s="36"/>
@@ -4658,7 +4658,7 @@
         <v>47</v>
       </c>
       <c r="H81" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I81" s="36"/>
       <c r="J81" s="36"/>
@@ -4677,7 +4677,7 @@
         <v>102</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I82" s="36"/>
       <c r="J82" s="36"/>
@@ -4696,7 +4696,7 @@
         <v>103</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I83" s="36"/>
       <c r="J83" s="36"/>
@@ -4715,7 +4715,7 @@
         <v>104</v>
       </c>
       <c r="H84" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I84" s="36"/>
       <c r="J84" s="36"/>
@@ -4734,7 +4734,7 @@
         <v>105</v>
       </c>
       <c r="H85" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I85" s="36"/>
       <c r="J85" s="36"/>
@@ -4753,7 +4753,7 @@
         <v>106</v>
       </c>
       <c r="H86" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I86" s="34"/>
       <c r="J86" s="34"/>
@@ -4806,10 +4806,10 @@
         <v>108</v>
       </c>
       <c r="H89" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="I89" s="32" t="s">
         <v>126</v>
-      </c>
-      <c r="I89" s="32" t="s">
-        <v>127</v>
       </c>
       <c r="J89" s="32" t="s">
         <v>143</v>
@@ -4829,7 +4829,7 @@
         <v>81</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I90" s="36"/>
       <c r="J90" s="36"/>
@@ -4848,7 +4848,7 @@
         <v>44</v>
       </c>
       <c r="H91" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I91" s="36"/>
       <c r="J91" s="36"/>
@@ -4869,7 +4869,7 @@
         <v>47</v>
       </c>
       <c r="H92" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I92" s="36"/>
       <c r="J92" s="36"/>
@@ -4890,7 +4890,7 @@
         <v>102</v>
       </c>
       <c r="H93" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I93" s="36"/>
       <c r="J93" s="36"/>
@@ -4909,7 +4909,7 @@
         <v>103</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I94" s="36"/>
       <c r="J94" s="36"/>
@@ -4928,7 +4928,7 @@
         <v>104</v>
       </c>
       <c r="H95" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I95" s="36"/>
       <c r="J95" s="36"/>
@@ -4947,7 +4947,7 @@
         <v>105</v>
       </c>
       <c r="H96" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I96" s="36"/>
       <c r="J96" s="36"/>
@@ -4966,7 +4966,7 @@
         <v>106</v>
       </c>
       <c r="H97" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I97" s="34"/>
       <c r="J97" s="34"/>
@@ -5021,7 +5021,7 @@
         <v>108</v>
       </c>
       <c r="H100" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I100" s="12" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
added leave rule list and db folder added
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -404,13 +404,13 @@
     <t>Holiday Management  Module</t>
   </si>
   <si>
+    <t>10-09-2023 to 12-09-2023</t>
+  </si>
+  <si>
+    <t>Leave Management  Module</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not done </t>
-  </si>
-  <si>
-    <t>10-09-2023 to 12-09-2023</t>
-  </si>
-  <si>
-    <t>Leave Management  Module</t>
   </si>
   <si>
     <t>3 Days</t>
@@ -2961,8 +2961,8 @@
   <sheetPr/>
   <dimension ref="A1:R114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I16"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3625,14 +3625,14 @@
       <c r="G29" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>129</v>
+      <c r="H29" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I29" s="32" t="s">
         <v>120</v>
       </c>
       <c r="J29" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -3648,8 +3648,8 @@
       <c r="G30" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>129</v>
+      <c r="H30" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
@@ -3682,7 +3682,7 @@
         <v>4</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -3702,7 +3702,7 @@
         <v>58</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I33" s="32" t="s">
         <v>132</v>
@@ -3725,7 +3725,7 @@
         <v>59</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I34" s="36"/>
       <c r="J34" s="36"/>
@@ -3744,7 +3744,7 @@
         <v>60</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I35" s="36"/>
       <c r="J35" s="36"/>
@@ -3765,7 +3765,7 @@
         <v>61</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I36" s="36"/>
       <c r="J36" s="36"/>
@@ -3784,7 +3784,7 @@
         <v>62</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I37" s="36"/>
       <c r="J37" s="36"/>
@@ -3805,7 +3805,7 @@
         <v>63</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -3864,7 +3864,7 @@
         <v>65</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I41" s="32" t="s">
         <v>126</v>
@@ -3889,7 +3889,7 @@
         <v>66</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I42" s="36"/>
       <c r="J42" s="36"/>
@@ -3910,7 +3910,7 @@
         <v>67</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I43" s="36"/>
       <c r="J43" s="36"/>
@@ -3931,7 +3931,7 @@
         <v>68</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I44" s="36"/>
       <c r="J44" s="36"/>
@@ -3952,7 +3952,7 @@
         <v>69</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I45" s="36"/>
       <c r="J45" s="36"/>
@@ -3973,7 +3973,7 @@
         <v>70</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I46" s="36"/>
       <c r="J46" s="36"/>
@@ -3994,7 +3994,7 @@
         <v>71</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I47" s="36"/>
       <c r="J47" s="36"/>
@@ -4015,7 +4015,7 @@
         <v>72</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I48" s="36"/>
       <c r="J48" s="36"/>
@@ -4036,7 +4036,7 @@
         <v>73</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
@@ -4095,7 +4095,7 @@
         <v>75</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I52" s="32" t="s">
         <v>132</v>
@@ -4120,7 +4120,7 @@
         <v>76</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I53" s="36"/>
       <c r="J53" s="36"/>
@@ -4141,7 +4141,7 @@
         <v>77</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I54" s="36"/>
       <c r="J54" s="36"/>
@@ -4162,7 +4162,7 @@
         <v>78</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I55" s="36"/>
       <c r="J55" s="36"/>
@@ -4183,7 +4183,7 @@
         <v>79</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I56" s="36"/>
       <c r="J56" s="36"/>
@@ -4204,7 +4204,7 @@
         <v>80</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I57" s="36"/>
       <c r="J57" s="36"/>
@@ -4225,7 +4225,7 @@
         <v>81</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
@@ -4331,7 +4331,7 @@
         <v>88</v>
       </c>
       <c r="H64" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I64" s="32" t="s">
         <v>132</v>
@@ -4354,7 +4354,7 @@
         <v>89</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
@@ -4373,7 +4373,7 @@
         <v>90</v>
       </c>
       <c r="H66" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I66" s="36"/>
       <c r="J66" s="36"/>
@@ -4392,7 +4392,7 @@
         <v>91</v>
       </c>
       <c r="H67" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I67" s="36"/>
       <c r="J67" s="36"/>
@@ -4411,7 +4411,7 @@
         <v>92</v>
       </c>
       <c r="H68" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I68" s="34"/>
       <c r="J68" s="34"/>
@@ -4464,7 +4464,7 @@
         <v>97</v>
       </c>
       <c r="H71" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I71" s="32" t="s">
         <v>126</v>
@@ -4487,7 +4487,7 @@
         <v>98</v>
       </c>
       <c r="H72" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I72" s="36"/>
       <c r="J72" s="36"/>
@@ -4506,7 +4506,7 @@
         <v>99</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I73" s="36"/>
       <c r="J73" s="36"/>
@@ -4525,7 +4525,7 @@
         <v>57</v>
       </c>
       <c r="H74" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I74" s="36"/>
       <c r="J74" s="36"/>
@@ -4544,7 +4544,7 @@
         <v>27</v>
       </c>
       <c r="H75" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I75" s="36"/>
       <c r="J75" s="36"/>
@@ -4563,7 +4563,7 @@
         <v>100</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I76" s="36"/>
       <c r="J76" s="36"/>
@@ -4582,7 +4582,7 @@
         <v>101</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I77" s="36"/>
       <c r="J77" s="36"/>
@@ -4601,7 +4601,7 @@
         <v>88</v>
       </c>
       <c r="H78" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I78" s="36"/>
       <c r="J78" s="36"/>
@@ -4620,7 +4620,7 @@
         <v>81</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I79" s="36"/>
       <c r="J79" s="36"/>
@@ -4639,7 +4639,7 @@
         <v>44</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I80" s="36"/>
       <c r="J80" s="36"/>
@@ -4658,7 +4658,7 @@
         <v>47</v>
       </c>
       <c r="H81" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I81" s="36"/>
       <c r="J81" s="36"/>
@@ -4677,7 +4677,7 @@
         <v>102</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I82" s="36"/>
       <c r="J82" s="36"/>
@@ -4696,7 +4696,7 @@
         <v>103</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I83" s="36"/>
       <c r="J83" s="36"/>
@@ -4715,7 +4715,7 @@
         <v>104</v>
       </c>
       <c r="H84" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I84" s="36"/>
       <c r="J84" s="36"/>
@@ -4734,7 +4734,7 @@
         <v>105</v>
       </c>
       <c r="H85" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I85" s="36"/>
       <c r="J85" s="36"/>
@@ -4753,7 +4753,7 @@
         <v>106</v>
       </c>
       <c r="H86" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I86" s="34"/>
       <c r="J86" s="34"/>
@@ -4806,7 +4806,7 @@
         <v>108</v>
       </c>
       <c r="H89" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I89" s="32" t="s">
         <v>126</v>
@@ -4829,7 +4829,7 @@
         <v>81</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I90" s="36"/>
       <c r="J90" s="36"/>
@@ -4848,7 +4848,7 @@
         <v>44</v>
       </c>
       <c r="H91" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I91" s="36"/>
       <c r="J91" s="36"/>
@@ -4869,7 +4869,7 @@
         <v>47</v>
       </c>
       <c r="H92" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I92" s="36"/>
       <c r="J92" s="36"/>
@@ -4890,7 +4890,7 @@
         <v>102</v>
       </c>
       <c r="H93" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I93" s="36"/>
       <c r="J93" s="36"/>
@@ -4909,7 +4909,7 @@
         <v>103</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I94" s="36"/>
       <c r="J94" s="36"/>
@@ -4928,7 +4928,7 @@
         <v>104</v>
       </c>
       <c r="H95" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I95" s="36"/>
       <c r="J95" s="36"/>
@@ -4947,7 +4947,7 @@
         <v>105</v>
       </c>
       <c r="H96" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I96" s="36"/>
       <c r="J96" s="36"/>
@@ -4966,7 +4966,7 @@
         <v>106</v>
       </c>
       <c r="H97" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I97" s="34"/>
       <c r="J97" s="34"/>
@@ -5021,7 +5021,7 @@
         <v>108</v>
       </c>
       <c r="H100" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I100" s="12" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
working on leave report
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -410,13 +410,13 @@
     <t>Leave Management  Module</t>
   </si>
   <si>
+    <t>3 Days</t>
+  </si>
+  <si>
+    <t>13-09-2023 to 16-09-2023</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not done </t>
-  </si>
-  <si>
-    <t>3 Days</t>
-  </si>
-  <si>
-    <t>13-09-2023 to 16-09-2023</t>
   </si>
   <si>
     <t>Rota Module</t>
@@ -2961,8 +2961,8 @@
   <sheetPr/>
   <dimension ref="A1:R114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29:H30"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3701,14 +3701,14 @@
       <c r="G33" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="I33" s="32" t="s">
+      <c r="J33" s="32" t="s">
         <v>132</v>
-      </c>
-      <c r="J33" s="32" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3724,8 +3724,8 @@
       <c r="G34" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="H34" s="12" t="s">
-        <v>131</v>
+      <c r="H34" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I34" s="36"/>
       <c r="J34" s="36"/>
@@ -3743,8 +3743,8 @@
       <c r="G35" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H35" s="12" t="s">
-        <v>131</v>
+      <c r="H35" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="I35" s="36"/>
       <c r="J35" s="36"/>
@@ -3765,7 +3765,7 @@
         <v>61</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I36" s="36"/>
       <c r="J36" s="36"/>
@@ -3784,7 +3784,7 @@
         <v>62</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I37" s="36"/>
       <c r="J37" s="36"/>
@@ -3805,7 +3805,7 @@
         <v>63</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -3864,7 +3864,7 @@
         <v>65</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I41" s="32" t="s">
         <v>126</v>
@@ -3889,7 +3889,7 @@
         <v>66</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I42" s="36"/>
       <c r="J42" s="36"/>
@@ -3910,7 +3910,7 @@
         <v>67</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I43" s="36"/>
       <c r="J43" s="36"/>
@@ -3931,7 +3931,7 @@
         <v>68</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I44" s="36"/>
       <c r="J44" s="36"/>
@@ -3952,7 +3952,7 @@
         <v>69</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I45" s="36"/>
       <c r="J45" s="36"/>
@@ -3973,7 +3973,7 @@
         <v>70</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I46" s="36"/>
       <c r="J46" s="36"/>
@@ -3994,7 +3994,7 @@
         <v>71</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I47" s="36"/>
       <c r="J47" s="36"/>
@@ -4015,7 +4015,7 @@
         <v>72</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I48" s="36"/>
       <c r="J48" s="36"/>
@@ -4036,7 +4036,7 @@
         <v>73</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
@@ -4095,10 +4095,10 @@
         <v>75</v>
       </c>
       <c r="H52" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="I52" s="32" t="s">
         <v>131</v>
-      </c>
-      <c r="I52" s="32" t="s">
-        <v>132</v>
       </c>
       <c r="J52" s="32" t="s">
         <v>137</v>
@@ -4120,7 +4120,7 @@
         <v>76</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I53" s="36"/>
       <c r="J53" s="36"/>
@@ -4141,7 +4141,7 @@
         <v>77</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I54" s="36"/>
       <c r="J54" s="36"/>
@@ -4162,7 +4162,7 @@
         <v>78</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I55" s="36"/>
       <c r="J55" s="36"/>
@@ -4183,7 +4183,7 @@
         <v>79</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I56" s="36"/>
       <c r="J56" s="36"/>
@@ -4204,7 +4204,7 @@
         <v>80</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I57" s="36"/>
       <c r="J57" s="36"/>
@@ -4225,7 +4225,7 @@
         <v>81</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
@@ -4331,10 +4331,10 @@
         <v>88</v>
       </c>
       <c r="H64" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I64" s="32" t="s">
         <v>131</v>
-      </c>
-      <c r="I64" s="32" t="s">
-        <v>132</v>
       </c>
       <c r="J64" s="32" t="s">
         <v>141</v>
@@ -4354,7 +4354,7 @@
         <v>89</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
@@ -4373,7 +4373,7 @@
         <v>90</v>
       </c>
       <c r="H66" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I66" s="36"/>
       <c r="J66" s="36"/>
@@ -4392,7 +4392,7 @@
         <v>91</v>
       </c>
       <c r="H67" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I67" s="36"/>
       <c r="J67" s="36"/>
@@ -4411,7 +4411,7 @@
         <v>92</v>
       </c>
       <c r="H68" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I68" s="34"/>
       <c r="J68" s="34"/>
@@ -4464,7 +4464,7 @@
         <v>97</v>
       </c>
       <c r="H71" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I71" s="32" t="s">
         <v>126</v>
@@ -4487,7 +4487,7 @@
         <v>98</v>
       </c>
       <c r="H72" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I72" s="36"/>
       <c r="J72" s="36"/>
@@ -4506,7 +4506,7 @@
         <v>99</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I73" s="36"/>
       <c r="J73" s="36"/>
@@ -4525,7 +4525,7 @@
         <v>57</v>
       </c>
       <c r="H74" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I74" s="36"/>
       <c r="J74" s="36"/>
@@ -4544,7 +4544,7 @@
         <v>27</v>
       </c>
       <c r="H75" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I75" s="36"/>
       <c r="J75" s="36"/>
@@ -4563,7 +4563,7 @@
         <v>100</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I76" s="36"/>
       <c r="J76" s="36"/>
@@ -4582,7 +4582,7 @@
         <v>101</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I77" s="36"/>
       <c r="J77" s="36"/>
@@ -4601,7 +4601,7 @@
         <v>88</v>
       </c>
       <c r="H78" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I78" s="36"/>
       <c r="J78" s="36"/>
@@ -4620,7 +4620,7 @@
         <v>81</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I79" s="36"/>
       <c r="J79" s="36"/>
@@ -4639,7 +4639,7 @@
         <v>44</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I80" s="36"/>
       <c r="J80" s="36"/>
@@ -4658,7 +4658,7 @@
         <v>47</v>
       </c>
       <c r="H81" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I81" s="36"/>
       <c r="J81" s="36"/>
@@ -4677,7 +4677,7 @@
         <v>102</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I82" s="36"/>
       <c r="J82" s="36"/>
@@ -4696,7 +4696,7 @@
         <v>103</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I83" s="36"/>
       <c r="J83" s="36"/>
@@ -4715,7 +4715,7 @@
         <v>104</v>
       </c>
       <c r="H84" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I84" s="36"/>
       <c r="J84" s="36"/>
@@ -4734,7 +4734,7 @@
         <v>105</v>
       </c>
       <c r="H85" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I85" s="36"/>
       <c r="J85" s="36"/>
@@ -4753,7 +4753,7 @@
         <v>106</v>
       </c>
       <c r="H86" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I86" s="34"/>
       <c r="J86" s="34"/>
@@ -4806,7 +4806,7 @@
         <v>108</v>
       </c>
       <c r="H89" s="29" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I89" s="32" t="s">
         <v>126</v>
@@ -4829,7 +4829,7 @@
         <v>81</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I90" s="36"/>
       <c r="J90" s="36"/>
@@ -4848,7 +4848,7 @@
         <v>44</v>
       </c>
       <c r="H91" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I91" s="36"/>
       <c r="J91" s="36"/>
@@ -4869,7 +4869,7 @@
         <v>47</v>
       </c>
       <c r="H92" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I92" s="36"/>
       <c r="J92" s="36"/>
@@ -4890,7 +4890,7 @@
         <v>102</v>
       </c>
       <c r="H93" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I93" s="36"/>
       <c r="J93" s="36"/>
@@ -4909,7 +4909,7 @@
         <v>103</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I94" s="36"/>
       <c r="J94" s="36"/>
@@ -4928,7 +4928,7 @@
         <v>104</v>
       </c>
       <c r="H95" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I95" s="36"/>
       <c r="J95" s="36"/>
@@ -4947,7 +4947,7 @@
         <v>105</v>
       </c>
       <c r="H96" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I96" s="36"/>
       <c r="J96" s="36"/>
@@ -4966,7 +4966,7 @@
         <v>106</v>
       </c>
       <c r="H97" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I97" s="34"/>
       <c r="J97" s="34"/>
@@ -5021,7 +5021,7 @@
         <v>108</v>
       </c>
       <c r="H100" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I100" s="12" t="s">
         <v>144</v>

</xml_diff>